<commit_message>
Split refabs into small, medium and large domain size
</commit_message>
<xml_diff>
--- a/bindingSites2Test.xlsx
+++ b/bindingSites2Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshyk/Desktop/reFABS-Procedure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC44C6-858E-6C44-90DC-F65668755BCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F695457-CC28-8646-BD8A-F072D7DD9A80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23720" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="32040" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:E1233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>